<commit_message>
Add .gitignore, update Excel paths, and implement email sending functionality
- Pending a change in the workflow. Card creation must be separated from email sending
</commit_message>
<xml_diff>
--- a/Docs/socios.xlsx
+++ b/Docs/socios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mierdas\github\workspace\harboroughSeasonTickets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA792AA8-654C-4FC4-873C-22C4450F71DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF20463-88AE-436F-8FB2-826E306B1213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{65BDEB92-D308-4CF4-9DB7-6064F5E6E16D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{65BDEB92-D308-4CF4-9DB7-6064F5E6E16D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>apellidos 1</t>
   </si>
   <si>
-    <t>test@lamediainglesa.com</t>
-  </si>
-  <si>
     <t>nombre2</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>nombre</t>
+  </si>
+  <si>
+    <t>joeljuaristi@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,23 +472,23 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -507,13 +507,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -521,13 +521,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -535,13 +535,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -549,13 +549,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -565,7 +565,10 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{C655E319-E980-436A-9E65-3589D5483F84}"/>
-    <hyperlink ref="C3:C6" r:id="rId2" display="test@lamediainglesa.com" xr:uid="{37F2739A-3058-491E-9E6A-EDEDFD19DD41}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{07C40A77-073D-4D23-9D8E-01E81F2FEC67}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{B6823D09-9D48-47C1-88B9-830B7A83DD60}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{76CFB26F-EA39-48A5-92D2-5D302E711720}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{2AD6F54F-2DEB-4A78-8933-90971AEF3D08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>